<commit_message>
final EP94 OS31 runs
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4_OS.xlsx
+++ b/results/RESULTS5-4_OS.xlsx
@@ -13795,7 +13795,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>09/30/2020</v>
+        <v>10/16/2020</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>55</v>
@@ -13834,7 +13834,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>10/01/2020</v>
+        <v>10/19/2020</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
Results for OpenStudio 3.5.1
Hold up was issue related to sql results missing for a few fields.
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4_OS.xlsx
+++ b/results/RESULTS5-4_OS.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>OpenStudio 3.5.0</v>
+        <v>OpenStudio 3.5.1</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>11/03/2022</v>
+        <v>12/29/2022</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>
@@ -14322,7 +14322,7 @@
       <c r="H5" s="349"/>
       <c r="I5" s="295"/>
       <c r="J5" s="360" t="str">
-        <v>11/03/2022</v>
+        <v>11/05/2024</v>
       </c>
       <c r="K5" s="109"/>
     </row>

</xml_diff>

<commit_message>
draft EP 24.2 OS 3.9
@dareumnam you fixed Unshaded Ann Trans and Shed Ann Trans results in 5-2a with OS 3.5, and that worked through 3.8, but those same values are gone again with 3.9? Any ideas of changes to E+ for 24.2 that I need to adjust for?
</commit_message>
<xml_diff>
--- a/results/RESULTS5-4_OS.xlsx
+++ b/results/RESULTS5-4_OS.xlsx
@@ -14264,7 +14264,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="377" t="str">
-        <v>OpenStudio 3.8.0</v>
+        <v>OpenStudio 3.9.0</v>
       </c>
       <c r="G2" s="378"/>
       <c r="H2" s="378"/>
@@ -14283,7 +14283,7 @@
       <c r="H3" s="349"/>
       <c r="I3" s="295"/>
       <c r="J3" s="360" t="str">
-        <v>5/18/2024</v>
+        <v>11/15/2024 (expected)</v>
       </c>
       <c r="K3" s="108" t="s">
         <v>54</v>

</xml_diff>